<commit_message>
Added channel, changed CAN transceiver, used NMOS
</commit_message>
<xml_diff>
--- a/Battery_Levelling/Battery_Leveling_Board_BOM.xlsx
+++ b/Battery_Levelling/Battery_Leveling_Board_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARVP\au_hardware\Battery_Levelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE9B8EF-2612-4758-8B9E-9A3F6FC6248A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4499BA-6D20-4D4D-8C0F-26CFD272C1BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12972" yWindow="2244" windowWidth="17280" windowHeight="8964" xr2:uid="{8382C762-F7B2-42A4-ACBF-DFFF73413A79}"/>
+    <workbookView xWindow="-11532" yWindow="828" windowWidth="17280" windowHeight="8964" xr2:uid="{8382C762-F7B2-42A4-ACBF-DFFF73413A79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>RES SMD 220 OHM 1% 1/8W 0805</t>
   </si>
@@ -50,9 +50,6 @@
     <t>RC0805FR-071KL</t>
   </si>
   <si>
-    <t>C4,5</t>
-  </si>
-  <si>
     <t>CAP CER 10UF 16V X7R 0805</t>
   </si>
   <si>
@@ -62,18 +59,6 @@
     <t>http://www.samsungsem.com/kr/support/product-search/mlcc/CL21B106KOQNNNG.jsp</t>
   </si>
   <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>IC TXRX CAN FAULT PROT 8SOIC</t>
-  </si>
-  <si>
-    <t>TCAN1042HVDRQ1</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tcan1042hgv-q1.pdf</t>
-  </si>
-  <si>
     <t>CON1</t>
   </si>
   <si>
@@ -140,9 +125,6 @@
     <t>R1,3</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
     <t>5V</t>
   </si>
   <si>
@@ -158,15 +140,6 @@
     <t>SM03B-GHS-TB(LF)(SN)</t>
   </si>
   <si>
-    <t>U$1-3</t>
-  </si>
-  <si>
-    <t>C1-3</t>
-  </si>
-  <si>
-    <t>U$4-6</t>
-  </si>
-  <si>
     <t>IC OR CTRLR N+1 6SOT</t>
   </si>
   <si>
@@ -209,45 +182,9 @@
     <t>TERM BLK 2P SIDE ENT 6.35MM PCB</t>
   </si>
   <si>
-    <t>J1-5</t>
-  </si>
-  <si>
-    <t>U$7</t>
-  </si>
-  <si>
-    <t>MOSFET P-CH 20V 60A PPAK SO-8</t>
-  </si>
-  <si>
-    <t>SI7157DP-T1-GE3</t>
-  </si>
-  <si>
-    <t>http://www.vishay.com/docs/62860/si7157dp.pdf</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>TRANS NPN 80V 1A SOT223</t>
-  </si>
-  <si>
-    <t>BCP56-16T1G</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pub/Collateral/BCP56T1-D.PDF</t>
-  </si>
-  <si>
-    <t>R5-7,10</t>
-  </si>
-  <si>
-    <t>RES SMD 5.1K OHM 5% 1/4W 1206</t>
-  </si>
-  <si>
-    <t>RC1206JR-075K1L</t>
-  </si>
-  <si>
     <t>Shematic Reference Number</t>
   </si>
   <si>
@@ -276,6 +213,90 @@
   </si>
   <si>
     <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>U2-5</t>
+  </si>
+  <si>
+    <t>C1-4</t>
+  </si>
+  <si>
+    <t>C5,6</t>
+  </si>
+  <si>
+    <t>Q1-4</t>
+  </si>
+  <si>
+    <t>R5-7,11</t>
+  </si>
+  <si>
+    <t>J1-6</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>MCP2562-E/SN</t>
+  </si>
+  <si>
+    <t>IC TRANSCEIVER HALF 1/1 8SOIC</t>
+  </si>
+  <si>
+    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/20005167C.pdf</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>IC GATE DRVR HI/LOW SIDE 8SOIC</t>
+  </si>
+  <si>
+    <t>IR2301SPBF‎</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>R9,10</t>
+  </si>
+  <si>
+    <t>RES SMD 5.1 OHM 5% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>‎RC1206JR-075R1L‎</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 50V X5R 1206</t>
+  </si>
+  <si>
+    <t>CL31A106MBHNNNE‎</t>
+  </si>
+  <si>
+    <t>CAP CER 1.5UF 50V JB 0805</t>
+  </si>
+  <si>
+    <t>C2012JB1H155M125AB‎</t>
+  </si>
+  <si>
+    <t>http://www.samsungsem.com/kr/support/product-search/mlcc/CL31A106MBHNNNE.jsp</t>
+  </si>
+  <si>
+    <t>https://product.tdk.com/info/en/catalog/datasheets/mlcc_commercial_general_en.pdf?ref_disty=digikey</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 1A DO214AC</t>
+  </si>
+  <si>
+    <t>‎CDBA140-G‎</t>
+  </si>
+  <si>
+    <t>http://www.comchiptech.com/admin/files/product/CDBA140-HF%20Thru192841.%20CDBA1100-HF%20RevB.pdf</t>
   </si>
 </sst>
 </file>
@@ -335,13 +356,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -657,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0087A257-B5F3-4283-A1EE-F066CFF45B21}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,39 +696,39 @@
   <sheetData>
     <row r="1" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -728,7 +751,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -751,16 +774,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
       </c>
       <c r="E4">
         <v>0.39</v>
@@ -774,19 +797,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
+        <v>67</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E5">
-        <v>2.0499999999999998</v>
+        <v>1.28</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -797,16 +820,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>39281023</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>0.83</v>
@@ -820,16 +843,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E7">
         <v>0.2</v>
@@ -843,16 +866,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>1.28</v>
@@ -866,16 +889,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E9">
         <v>0.46</v>
@@ -889,16 +912,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>0.5</v>
@@ -912,13 +935,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -935,16 +958,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E12">
         <v>0.68</v>
@@ -958,88 +981,88 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E13">
         <v>3.56</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I13">
-        <f>F13*E13</f>
-        <v>10.68</v>
+        <f t="shared" ref="I13:I22" si="0">F13*E13</f>
+        <v>14.24</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <v>0.16</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <f>F14*E14</f>
-        <v>0.48</v>
+        <f t="shared" si="0"/>
+        <v>0.64</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="E15">
         <v>2.1800000000000002</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15">
-        <f>F15*E15</f>
-        <v>6.5400000000000009</v>
+        <f t="shared" si="0"/>
+        <v>8.7200000000000006</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E16">
         <v>0.15</v>
@@ -1048,104 +1071,152 @@
         <v>4</v>
       </c>
       <c r="I16">
-        <f>F16*E16</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C17">
         <v>1714955</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E17">
         <v>2.46</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I17">
-        <f>F17*E17</f>
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>14.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2.71</v>
+      </c>
+      <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="I18">
-        <f>F18*E18</f>
-        <v>2.1800000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19">
-        <v>0.15</v>
-      </c>
-      <c r="F19">
+      <c r="I18" s="4">
+        <f t="shared" si="0"/>
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="F19" s="4">
         <v>1</v>
       </c>
-      <c r="I19">
-        <f>F19*E19</f>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20">
-        <v>0.59</v>
-      </c>
-      <c r="F20">
+      <c r="I19" s="4">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="I20">
-        <f>F20*E20</f>
-        <v>0.59</v>
+      <c r="I20" s="4">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
       </c>
     </row>
   </sheetData>
@@ -1155,9 +1226,9 @@
     <hyperlink ref="D15" r:id="rId3" xr:uid="{88A1A547-CA3C-4F86-A243-80C60026F7F7}"/>
     <hyperlink ref="D16" r:id="rId4" xr:uid="{D7075404-BD0E-4300-A6F4-A693DD466BF6}"/>
     <hyperlink ref="D17" r:id="rId5" display="https://media.digikey.com/pdf/Data Sheets/Phoenix Contact PDFs/1714955.pdf" xr:uid="{EB8640F4-9DE4-45B1-94F3-22532BFF91B0}"/>
-    <hyperlink ref="D18" r:id="rId6" xr:uid="{0D3342E1-21E6-4A3B-B121-F660C218A79A}"/>
-    <hyperlink ref="D20" r:id="rId7" xr:uid="{34AB8669-2B95-460C-A872-E205853B4CAB}"/>
-    <hyperlink ref="D19" r:id="rId8" xr:uid="{BCD14FD1-BFF1-49B4-8FF8-DC769E8BBD7D}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{833BA616-3513-4A8B-BB62-CFBEC8C57757}"/>
+    <hyperlink ref="D18" r:id="rId7" xr:uid="{358D1B73-0305-4650-B506-EAAFBC50DEA9}"/>
+    <hyperlink ref="D22" r:id="rId8" display="http://www.comchiptech.com/admin/files/product/CDBA140-HF Thru192841. CDBA1100-HF RevB.pdf" xr:uid="{CF256C89-180E-4EC4-9430-C7D2F4CE7D88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>

</xml_diff>

<commit_message>
Added PCB board file for battery levelling board
</commit_message>
<xml_diff>
--- a/Battery_Levelling/Battery_Leveling_Board_BOM.xlsx
+++ b/Battery_Levelling/Battery_Leveling_Board_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARVP\au_hardware\Battery_Levelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4499BA-6D20-4D4D-8C0F-26CFD272C1BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8395F6B7-B13F-43ED-B4E9-6B55F0C290DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11532" yWindow="828" windowWidth="17280" windowHeight="8964" xr2:uid="{8382C762-F7B2-42A4-ACBF-DFFF73413A79}"/>
+    <workbookView xWindow="-10284" yWindow="5436" windowWidth="17280" windowHeight="8964" xr2:uid="{8382C762-F7B2-42A4-ACBF-DFFF73413A79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
   <si>
     <t>RES SMD 220 OHM 1% 1/8W 0805</t>
   </si>
@@ -68,9 +68,6 @@
     <t>http://www.molex.com/pdm_docs/sd/039281023_sd.pdf</t>
   </si>
   <si>
-    <t>SIL VERTICAL PC TAIL PIN HEADER 1x2</t>
-  </si>
-  <si>
     <t>M20-9990245</t>
   </si>
   <si>
@@ -297,6 +294,21 @@
   </si>
   <si>
     <t>http://www.comchiptech.com/admin/files/product/CDBA140-HF%20Thru192841.%20CDBA1100-HF%20RevB.pdf</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 20V 21A 8-TSSOP</t>
+  </si>
+  <si>
+    <t>DMN2011UTS-13</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/DMN2011UTS.pdf</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 2POS</t>
   </si>
 </sst>
 </file>
@@ -680,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0087A257-B5F3-4283-A1EE-F066CFF45B21}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,39 +708,39 @@
   <sheetData>
     <row r="1" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>29</v>
+      <c r="A2" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -750,8 +762,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>76</v>
+      <c r="A3" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -773,8 +785,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>62</v>
+      <c r="A4" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -796,17 +808,17 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="E5">
         <v>1.28</v>
@@ -819,7 +831,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
@@ -842,17 +854,17 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>28</v>
+      <c r="A7" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
       <c r="E7">
         <v>0.2</v>
@@ -865,17 +877,17 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
       </c>
       <c r="E8">
         <v>1.28</v>
@@ -888,17 +900,17 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>30</v>
+      <c r="A9" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
       <c r="E9">
         <v>0.46</v>
@@ -911,17 +923,17 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
       </c>
       <c r="E10">
         <v>0.5</v>
@@ -934,14 +946,14 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>31</v>
+      <c r="A11" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -957,17 +969,17 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12">
         <v>0.68</v>
@@ -980,17 +992,17 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>60</v>
+      <c r="A13" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="E13">
         <v>3.56</v>
@@ -999,22 +1011,22 @@
         <v>4</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:I22" si="0">F13*E13</f>
+        <f t="shared" ref="I13:I23" si="0">F13*E13</f>
         <v>14.24</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>61</v>
+      <c r="A14" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="E14">
         <v>0.16</v>
@@ -1028,17 +1040,17 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>63</v>
+      <c r="A15" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E15">
         <v>2.1800000000000002</v>
@@ -1052,17 +1064,17 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>64</v>
+      <c r="A16" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="E16">
         <v>0.15</v>
@@ -1076,17 +1088,17 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>65</v>
+      <c r="A17" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17">
         <v>1714955</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17">
         <v>2.46</v>
@@ -1101,16 +1113,16 @@
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E18" s="4">
         <v>2.71</v>
@@ -1125,16 +1137,16 @@
     </row>
     <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="4">
         <v>0.18</v>
@@ -1149,16 +1161,16 @@
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" s="4">
         <v>0.47</v>
@@ -1173,16 +1185,16 @@
     </row>
     <row r="21" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="4">
         <v>0.76</v>
@@ -1197,16 +1209,16 @@
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="E22" s="4">
         <v>0.49</v>
@@ -1217,6 +1229,30 @@
       <c r="I22" s="4">
         <f t="shared" si="0"/>
         <v>0.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="0"/>
+        <v>0.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>